<commit_message>
Update poll and report link
</commit_message>
<xml_diff>
--- a/doc/poll_analysis.xlsx
+++ b/doc/poll_analysis.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="I:\OSU\conference\UCGIS_2020\UCGIS-Fullstack-Geovisualization-Workshop\doc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F0638D1C-486E-4FDC-8101-A624662D123E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8D2DE10F-82DC-4896-B0E5-1CE23A3691BA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-23148" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="postworkshop" sheetId="2" r:id="rId1"/>
@@ -509,371 +509,587 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5A690A76-D742-4334-9A1F-B90EE0422D8A}">
-  <dimension ref="A1:K10"/>
+  <dimension ref="A1:S10"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D18" sqref="D18"/>
+    <sheetView tabSelected="1" topLeftCell="K1" workbookViewId="0">
+      <selection activeCell="S1" sqref="S1:S1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="8.85546875" customWidth="1"/>
-    <col min="2" max="2" width="19.140625" customWidth="1"/>
-    <col min="3" max="3" width="22.42578125" customWidth="1"/>
-    <col min="4" max="4" width="20" customWidth="1"/>
-    <col min="5" max="5" width="16" customWidth="1"/>
-    <col min="6" max="6" width="20.140625" customWidth="1"/>
-    <col min="7" max="7" width="18.5703125" customWidth="1"/>
-    <col min="8" max="8" width="21.5703125" customWidth="1"/>
-    <col min="9" max="9" width="23" customWidth="1"/>
-    <col min="10" max="10" width="18.42578125" customWidth="1"/>
-    <col min="11" max="11" width="17.5703125" customWidth="1"/>
+    <col min="2" max="3" width="19.140625" customWidth="1"/>
+    <col min="4" max="5" width="22.42578125" customWidth="1"/>
+    <col min="6" max="7" width="20" customWidth="1"/>
+    <col min="8" max="9" width="16" customWidth="1"/>
+    <col min="10" max="11" width="20.140625" customWidth="1"/>
+    <col min="12" max="13" width="18.5703125" customWidth="1"/>
+    <col min="14" max="15" width="21.5703125" customWidth="1"/>
+    <col min="16" max="17" width="23" customWidth="1"/>
+    <col min="18" max="18" width="18.42578125" customWidth="1"/>
+    <col min="19" max="19" width="17.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" s="1" customFormat="1" ht="99.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:19" s="1" customFormat="1" ht="99.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B1" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="D1" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="F1" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="H1" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="J1" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="L1" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="N1" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="P1" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="J1" s="1" t="s">
+      <c r="R1" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="K1" s="1" t="s">
+      <c r="S1" s="1" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1</v>
       </c>
       <c r="B2" t="s">
         <v>11</v>
       </c>
-      <c r="C2" t="s">
+      <c r="C2">
+        <v>4</v>
+      </c>
+      <c r="D2" t="s">
         <v>11</v>
       </c>
-      <c r="D2" t="s">
+      <c r="E2">
+        <v>4</v>
+      </c>
+      <c r="F2" t="s">
         <v>14</v>
       </c>
-      <c r="E2" t="s">
+      <c r="G2">
+        <v>4</v>
+      </c>
+      <c r="H2" t="s">
         <v>16</v>
       </c>
-      <c r="F2" t="s">
+      <c r="I2">
+        <v>5</v>
+      </c>
+      <c r="J2" t="s">
         <v>18</v>
       </c>
-      <c r="G2" t="s">
+      <c r="K2">
+        <v>5</v>
+      </c>
+      <c r="L2" t="s">
         <v>22</v>
       </c>
-      <c r="H2" t="s">
+      <c r="M2">
+        <v>3</v>
+      </c>
+      <c r="N2" t="s">
         <v>38</v>
       </c>
-      <c r="I2" t="s">
+      <c r="O2">
+        <v>4</v>
+      </c>
+      <c r="P2" t="s">
         <v>42</v>
       </c>
-      <c r="J2" t="s">
-        <v>9</v>
-      </c>
-      <c r="K2" t="s">
+      <c r="Q2">
+        <v>3</v>
+      </c>
+      <c r="R2" t="s">
+        <v>9</v>
+      </c>
+      <c r="S2" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>2</v>
       </c>
       <c r="B3" t="s">
         <v>5</v>
       </c>
-      <c r="C3" t="s">
+      <c r="C3">
         <v>5</v>
       </c>
       <c r="D3" t="s">
+        <v>5</v>
+      </c>
+      <c r="E3">
+        <v>5</v>
+      </c>
+      <c r="F3" t="s">
         <v>16</v>
       </c>
-      <c r="E3" t="s">
+      <c r="G3">
+        <v>5</v>
+      </c>
+      <c r="H3" t="s">
         <v>16</v>
       </c>
-      <c r="F3" t="s">
+      <c r="I3">
+        <v>5</v>
+      </c>
+      <c r="J3" t="s">
         <v>18</v>
       </c>
-      <c r="G3" t="s">
-        <v>5</v>
-      </c>
-      <c r="H3" t="s">
+      <c r="K3">
+        <v>5</v>
+      </c>
+      <c r="L3" t="s">
+        <v>5</v>
+      </c>
+      <c r="M3">
+        <v>5</v>
+      </c>
+      <c r="N3" t="s">
         <v>39</v>
       </c>
-      <c r="I3" t="s">
+      <c r="O3">
+        <v>5</v>
+      </c>
+      <c r="P3" t="s">
         <v>43</v>
       </c>
-      <c r="J3" t="s">
+      <c r="Q3">
+        <v>5</v>
+      </c>
+      <c r="R3" t="s">
         <v>16</v>
       </c>
-      <c r="K3" t="s">
+      <c r="S3" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>3</v>
       </c>
       <c r="B4" t="s">
         <v>11</v>
       </c>
-      <c r="C4" t="s">
-        <v>5</v>
+      <c r="C4">
+        <v>4</v>
       </c>
       <c r="D4" t="s">
+        <v>5</v>
+      </c>
+      <c r="E4">
+        <v>5</v>
+      </c>
+      <c r="F4" t="s">
         <v>16</v>
       </c>
-      <c r="E4" t="s">
+      <c r="G4">
+        <v>5</v>
+      </c>
+      <c r="H4" t="s">
         <v>16</v>
       </c>
-      <c r="F4" t="s">
+      <c r="I4">
+        <v>5</v>
+      </c>
+      <c r="J4" t="s">
         <v>18</v>
       </c>
-      <c r="G4" t="s">
-        <v>5</v>
-      </c>
-      <c r="H4" t="s">
+      <c r="K4">
+        <v>5</v>
+      </c>
+      <c r="L4" t="s">
+        <v>5</v>
+      </c>
+      <c r="M4">
+        <v>5</v>
+      </c>
+      <c r="N4" t="s">
         <v>38</v>
       </c>
-      <c r="I4" t="s">
+      <c r="O4">
+        <v>4</v>
+      </c>
+      <c r="P4" t="s">
         <v>44</v>
       </c>
-      <c r="J4" t="s">
-        <v>9</v>
-      </c>
-      <c r="K4" t="s">
+      <c r="Q4">
+        <v>4</v>
+      </c>
+      <c r="R4" t="s">
+        <v>9</v>
+      </c>
+      <c r="S4" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>4</v>
       </c>
       <c r="B5" t="s">
         <v>5</v>
       </c>
-      <c r="C5" t="s">
+      <c r="C5">
         <v>5</v>
       </c>
       <c r="D5" t="s">
+        <v>5</v>
+      </c>
+      <c r="E5">
+        <v>5</v>
+      </c>
+      <c r="F5" t="s">
         <v>16</v>
       </c>
-      <c r="E5" t="s">
+      <c r="G5">
+        <v>5</v>
+      </c>
+      <c r="H5" t="s">
         <v>14</v>
       </c>
-      <c r="F5" t="s">
+      <c r="I5">
+        <v>4</v>
+      </c>
+      <c r="J5" t="s">
         <v>29</v>
       </c>
-      <c r="G5" t="s">
-        <v>5</v>
-      </c>
-      <c r="H5" t="s">
+      <c r="K5">
+        <v>4</v>
+      </c>
+      <c r="L5" t="s">
+        <v>5</v>
+      </c>
+      <c r="M5">
+        <v>5</v>
+      </c>
+      <c r="N5" t="s">
         <v>39</v>
       </c>
-      <c r="I5" t="s">
+      <c r="O5">
+        <v>5</v>
+      </c>
+      <c r="P5" t="s">
         <v>43</v>
       </c>
-      <c r="J5" t="s">
-        <v>9</v>
-      </c>
-      <c r="K5" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="Q5">
+        <v>5</v>
+      </c>
+      <c r="R5" t="s">
+        <v>9</v>
+      </c>
+      <c r="S5" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="6" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>5</v>
       </c>
       <c r="B6" t="s">
         <v>30</v>
       </c>
-      <c r="C6" t="s">
+      <c r="C6">
+        <v>2</v>
+      </c>
+      <c r="D6" t="s">
         <v>22</v>
       </c>
-      <c r="D6" t="s">
+      <c r="E6">
+        <v>3</v>
+      </c>
+      <c r="F6" t="s">
         <v>16</v>
       </c>
-      <c r="E6" t="s">
+      <c r="G6">
+        <v>5</v>
+      </c>
+      <c r="H6" t="s">
         <v>14</v>
       </c>
-      <c r="F6" t="s">
+      <c r="I6">
+        <v>4</v>
+      </c>
+      <c r="J6" t="s">
         <v>31</v>
       </c>
-      <c r="G6" t="s">
-        <v>5</v>
-      </c>
-      <c r="H6" t="s">
+      <c r="K6">
+        <v>3</v>
+      </c>
+      <c r="L6" t="s">
+        <v>5</v>
+      </c>
+      <c r="M6">
+        <v>5</v>
+      </c>
+      <c r="N6" t="s">
         <v>40</v>
       </c>
-      <c r="I6" t="s">
+      <c r="O6">
+        <v>3</v>
+      </c>
+      <c r="P6" t="s">
         <v>42</v>
       </c>
-      <c r="J6" t="s">
+      <c r="Q6">
+        <v>3</v>
+      </c>
+      <c r="R6" t="s">
         <v>23</v>
       </c>
-      <c r="K6" t="s">
+      <c r="S6" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>6</v>
       </c>
       <c r="B7" t="s">
         <v>11</v>
       </c>
-      <c r="C7" t="s">
+      <c r="C7">
+        <v>4</v>
+      </c>
+      <c r="D7" t="s">
         <v>11</v>
       </c>
-      <c r="D7" t="s">
+      <c r="E7">
+        <v>4</v>
+      </c>
+      <c r="F7" t="s">
         <v>14</v>
       </c>
-      <c r="E7" t="s">
+      <c r="G7">
+        <v>4</v>
+      </c>
+      <c r="H7" t="s">
         <v>16</v>
       </c>
-      <c r="F7" t="s">
+      <c r="I7">
+        <v>5</v>
+      </c>
+      <c r="J7" t="s">
         <v>18</v>
       </c>
-      <c r="G7" t="s">
+      <c r="K7">
+        <v>5</v>
+      </c>
+      <c r="L7" t="s">
         <v>11</v>
       </c>
-      <c r="H7" t="s">
+      <c r="M7">
+        <v>4</v>
+      </c>
+      <c r="N7" t="s">
         <v>40</v>
       </c>
-      <c r="I7" t="s">
+      <c r="O7">
+        <v>3</v>
+      </c>
+      <c r="P7" t="s">
         <v>44</v>
       </c>
-      <c r="J7" t="s">
+      <c r="Q7">
+        <v>4</v>
+      </c>
+      <c r="R7" t="s">
         <v>14</v>
       </c>
-      <c r="K7" t="s">
+      <c r="S7" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>7</v>
       </c>
       <c r="B8" t="s">
         <v>11</v>
       </c>
-      <c r="C8" t="s">
+      <c r="C8">
+        <v>4</v>
+      </c>
+      <c r="D8" t="s">
         <v>11</v>
       </c>
-      <c r="D8" t="s">
+      <c r="E8">
+        <v>4</v>
+      </c>
+      <c r="F8" t="s">
         <v>16</v>
       </c>
-      <c r="E8" t="s">
+      <c r="G8">
+        <v>5</v>
+      </c>
+      <c r="H8" t="s">
         <v>14</v>
       </c>
-      <c r="F8" t="s">
+      <c r="I8">
+        <v>4</v>
+      </c>
+      <c r="J8" t="s">
         <v>18</v>
       </c>
-      <c r="G8" t="s">
-        <v>5</v>
-      </c>
-      <c r="H8" t="s">
+      <c r="K8">
+        <v>5</v>
+      </c>
+      <c r="L8" t="s">
+        <v>5</v>
+      </c>
+      <c r="M8">
+        <v>5</v>
+      </c>
+      <c r="N8" t="s">
         <v>39</v>
       </c>
-      <c r="I8" t="s">
+      <c r="O8">
+        <v>5</v>
+      </c>
+      <c r="P8" t="s">
         <v>44</v>
       </c>
-      <c r="J8" t="s">
-        <v>9</v>
-      </c>
-      <c r="K8" t="s">
+      <c r="Q8">
+        <v>4</v>
+      </c>
+      <c r="R8" t="s">
+        <v>9</v>
+      </c>
+      <c r="S8" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>8</v>
       </c>
       <c r="B9" t="s">
         <v>5</v>
       </c>
-      <c r="C9" t="s">
+      <c r="C9">
         <v>5</v>
       </c>
       <c r="D9" t="s">
+        <v>5</v>
+      </c>
+      <c r="E9">
+        <v>5</v>
+      </c>
+      <c r="F9" t="s">
         <v>16</v>
       </c>
-      <c r="E9" t="s">
+      <c r="G9">
+        <v>5</v>
+      </c>
+      <c r="H9" t="s">
         <v>14</v>
       </c>
-      <c r="F9" t="s">
+      <c r="I9">
+        <v>4</v>
+      </c>
+      <c r="J9" t="s">
         <v>18</v>
       </c>
-      <c r="G9" t="s">
-        <v>5</v>
-      </c>
-      <c r="H9" t="s">
+      <c r="K9">
+        <v>5</v>
+      </c>
+      <c r="L9" t="s">
+        <v>5</v>
+      </c>
+      <c r="M9">
+        <v>5</v>
+      </c>
+      <c r="N9" t="s">
         <v>39</v>
       </c>
-      <c r="I9" t="s">
+      <c r="O9">
+        <v>5</v>
+      </c>
+      <c r="P9" t="s">
         <v>42</v>
       </c>
-      <c r="J9" t="s">
-        <v>9</v>
-      </c>
-      <c r="K9" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="Q9">
+        <v>3</v>
+      </c>
+      <c r="R9" t="s">
+        <v>9</v>
+      </c>
+      <c r="S9" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="10" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>9</v>
       </c>
       <c r="B10" t="s">
         <v>5</v>
       </c>
-      <c r="C10" t="s">
+      <c r="C10">
         <v>5</v>
       </c>
       <c r="D10" t="s">
+        <v>5</v>
+      </c>
+      <c r="E10">
+        <v>5</v>
+      </c>
+      <c r="F10" t="s">
         <v>14</v>
       </c>
-      <c r="E10" t="s">
+      <c r="G10">
+        <v>4</v>
+      </c>
+      <c r="H10" t="s">
         <v>16</v>
       </c>
-      <c r="F10" t="s">
+      <c r="I10">
+        <v>5</v>
+      </c>
+      <c r="J10" t="s">
         <v>18</v>
       </c>
-      <c r="G10" t="s">
-        <v>5</v>
-      </c>
-      <c r="H10" t="s">
+      <c r="K10">
+        <v>5</v>
+      </c>
+      <c r="L10" t="s">
+        <v>5</v>
+      </c>
+      <c r="M10">
+        <v>5</v>
+      </c>
+      <c r="N10" t="s">
         <v>38</v>
       </c>
-      <c r="I10" t="s">
+      <c r="O10">
+        <v>4</v>
+      </c>
+      <c r="P10" t="s">
         <v>44</v>
       </c>
-      <c r="J10" t="s">
-        <v>9</v>
-      </c>
-      <c r="K10" t="s">
+      <c r="Q10">
+        <v>4</v>
+      </c>
+      <c r="R10" t="s">
+        <v>9</v>
+      </c>
+      <c r="S10" t="s">
         <v>46</v>
       </c>
     </row>
@@ -887,7 +1103,7 @@
   <dimension ref="A1:F8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F2" sqref="F2:F8"/>
+      <selection activeCell="H17" sqref="H17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1066,7 +1282,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0D45B27F-E4B3-40E5-B456-3FCDD7C010F5}">
   <dimension ref="B1:J11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView topLeftCell="B1" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
       <selection activeCell="N9" sqref="N9"/>
     </sheetView>
   </sheetViews>

</xml_diff>